<commit_message>
Creacion de Carpetas en el Backend y Tablas TP
</commit_message>
<xml_diff>
--- a/Formulario - Base de datos.xlsx
+++ b/Formulario - Base de datos.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3130" uniqueCount="488">
   <si>
     <t>Gobernacion maritima</t>
   </si>
@@ -1067,9 +1067,6 @@
     <t>FCInicioDenuncia</t>
   </si>
   <si>
-    <t>CDTPLugarProcedimiento</t>
-  </si>
-  <si>
     <t>GLTPLugarProcedimiento</t>
   </si>
   <si>
@@ -1476,6 +1473,15 @@
   </si>
   <si>
     <t>Funcionarios</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>LGSexoMasculino</t>
+  </si>
+  <si>
+    <t>Personas.PersonaNatural</t>
   </si>
 </sst>
 </file>
@@ -9564,8 +9570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D235" sqref="D235"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9596,6 +9602,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>485</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -9604,6 +9613,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>485</v>
+      </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -9612,6 +9624,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>485</v>
+      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -9620,20 +9635,26 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>485</v>
+      </c>
       <c r="B5" t="s">
         <v>294</v>
       </c>
       <c r="C5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D5" t="s">
         <v>343</v>
       </c>
       <c r="E5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>485</v>
+      </c>
       <c r="B6" t="s">
         <v>295</v>
       </c>
@@ -9641,13 +9662,16 @@
         <v>346</v>
       </c>
       <c r="D6" t="s">
+        <v>350</v>
+      </c>
+      <c r="E6" t="s">
         <v>351</v>
       </c>
-      <c r="E6" t="s">
-        <v>352</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>485</v>
+      </c>
       <c r="B7" t="s">
         <v>342</v>
       </c>
@@ -9659,6 +9683,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>485</v>
+      </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -9670,6 +9697,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>485</v>
+      </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -9681,25 +9711,31 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>485</v>
+      </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D10" t="s">
         <v>215</v>
       </c>
       <c r="E10" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>485</v>
+      </c>
       <c r="B11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9710,7 +9746,7 @@
         <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9721,13 +9757,13 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E14" t="s">
         <v>359</v>
-      </c>
-      <c r="D14" t="s">
-        <v>358</v>
-      </c>
-      <c r="E14" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9738,13 +9774,13 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9755,13 +9791,13 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9772,13 +9808,13 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D17" t="s">
         <v>215</v>
       </c>
       <c r="E17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9789,10 +9825,10 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
+        <v>363</v>
+      </c>
+      <c r="D18" t="s">
         <v>364</v>
-      </c>
-      <c r="D18" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9803,10 +9839,10 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9817,10 +9853,10 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9831,10 +9867,10 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E21" t="s">
         <v>293</v>
@@ -9848,10 +9884,10 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -9862,10 +9898,10 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -9876,7 +9912,7 @@
         <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -9887,7 +9923,7 @@
         <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -9898,7 +9934,7 @@
         <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -9909,10 +9945,10 @@
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -9923,10 +9959,10 @@
         <v>302</v>
       </c>
       <c r="C28" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -9937,10 +9973,10 @@
         <v>304</v>
       </c>
       <c r="C29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -9951,7 +9987,10 @@
         <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>376</v>
+        <v>375</v>
+      </c>
+      <c r="F31" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -9962,10 +10001,10 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
+        <v>376</v>
+      </c>
+      <c r="D32" t="s">
         <v>377</v>
-      </c>
-      <c r="D32" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -9976,7 +10015,10 @@
         <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>379</v>
+        <v>378</v>
+      </c>
+      <c r="F33" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -9987,7 +10029,10 @@
         <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>380</v>
+        <v>379</v>
+      </c>
+      <c r="F34" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -9998,7 +10043,10 @@
         <v>129</v>
       </c>
       <c r="E35" t="s">
-        <v>448</v>
+        <v>447</v>
+      </c>
+      <c r="F35" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -10006,10 +10054,13 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E36" t="s">
-        <v>449</v>
+        <v>448</v>
+      </c>
+      <c r="F36" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -10020,13 +10071,13 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
+        <v>381</v>
+      </c>
+      <c r="D37" t="s">
+        <v>380</v>
+      </c>
+      <c r="E37" t="s">
         <v>382</v>
-      </c>
-      <c r="D37" t="s">
-        <v>381</v>
-      </c>
-      <c r="E37" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -10037,7 +10088,10 @@
         <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>450</v>
+        <v>449</v>
+      </c>
+      <c r="F38" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -10048,13 +10102,13 @@
         <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D39" t="s">
         <v>213</v>
       </c>
       <c r="E39" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -10065,13 +10119,13 @@
         <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D40" t="s">
         <v>211</v>
       </c>
       <c r="E40" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -10081,8 +10135,14 @@
       <c r="B41" t="s">
         <v>63</v>
       </c>
+      <c r="C41" t="s">
+        <v>486</v>
+      </c>
+      <c r="D41" t="s">
+        <v>487</v>
+      </c>
       <c r="F41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -10093,13 +10153,13 @@
         <v>68</v>
       </c>
       <c r="C42" t="s">
+        <v>387</v>
+      </c>
+      <c r="D42" t="s">
         <v>388</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>389</v>
-      </c>
-      <c r="E42" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -10110,10 +10170,10 @@
         <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -10124,13 +10184,13 @@
         <v>67</v>
       </c>
       <c r="C44" t="s">
+        <v>391</v>
+      </c>
+      <c r="D44" t="s">
         <v>392</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>393</v>
-      </c>
-      <c r="E44" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -10141,7 +10201,7 @@
         <v>65</v>
       </c>
       <c r="F45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -10152,7 +10212,7 @@
         <v>66</v>
       </c>
       <c r="F46" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -10163,13 +10223,13 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
+        <v>395</v>
+      </c>
+      <c r="D47" t="s">
         <v>396</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>397</v>
-      </c>
-      <c r="E47" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -10180,10 +10240,10 @@
         <v>31</v>
       </c>
       <c r="C48" t="s">
+        <v>363</v>
+      </c>
+      <c r="D48" t="s">
         <v>364</v>
-      </c>
-      <c r="D48" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -10194,10 +10254,10 @@
         <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D49" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -10208,10 +10268,10 @@
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -10222,10 +10282,10 @@
         <v>34</v>
       </c>
       <c r="C51" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D51" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E51" t="s">
         <v>293</v>
@@ -10239,10 +10299,10 @@
         <v>35</v>
       </c>
       <c r="C52" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D52" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -10253,10 +10313,10 @@
         <v>36</v>
       </c>
       <c r="C53" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -10267,7 +10327,7 @@
         <v>37</v>
       </c>
       <c r="E54" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -10278,7 +10338,7 @@
         <v>38</v>
       </c>
       <c r="E55" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -10289,7 +10349,7 @@
         <v>39</v>
       </c>
       <c r="F56" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -10300,10 +10360,10 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D57" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -10387,13 +10447,13 @@
         <v>77</v>
       </c>
       <c r="C63" t="s">
+        <v>398</v>
+      </c>
+      <c r="D63" t="s">
+        <v>398</v>
+      </c>
+      <c r="E63" t="s">
         <v>399</v>
-      </c>
-      <c r="D63" t="s">
-        <v>399</v>
-      </c>
-      <c r="E63" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -10404,10 +10464,10 @@
         <v>323</v>
       </c>
       <c r="C64" t="s">
+        <v>400</v>
+      </c>
+      <c r="D64" t="s">
         <v>401</v>
-      </c>
-      <c r="D64" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -10415,16 +10475,16 @@
         <v>49</v>
       </c>
       <c r="B65" t="s">
+        <v>403</v>
+      </c>
+      <c r="C65" t="s">
         <v>404</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>405</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>406</v>
-      </c>
-      <c r="E65" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -10435,13 +10495,13 @@
         <v>78</v>
       </c>
       <c r="C66" t="s">
+        <v>407</v>
+      </c>
+      <c r="D66" t="s">
         <v>408</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>409</v>
-      </c>
-      <c r="E66" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -10452,10 +10512,10 @@
         <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D67" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -10466,16 +10526,16 @@
         <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D68" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E68" t="s">
         <v>328</v>
       </c>
       <c r="F68" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -10489,13 +10549,13 @@
         <v>326</v>
       </c>
       <c r="D69" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E69" t="s">
         <v>328</v>
       </c>
       <c r="F69" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -10509,13 +10569,13 @@
         <v>325</v>
       </c>
       <c r="D70" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E70" t="s">
         <v>328</v>
       </c>
       <c r="F70" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -10526,13 +10586,13 @@
         <v>194</v>
       </c>
       <c r="C72" t="s">
+        <v>412</v>
+      </c>
+      <c r="D72" t="s">
         <v>413</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>414</v>
-      </c>
-      <c r="E72" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -10543,10 +10603,10 @@
         <v>94</v>
       </c>
       <c r="C73" t="s">
+        <v>415</v>
+      </c>
+      <c r="D73" t="s">
         <v>416</v>
-      </c>
-      <c r="D73" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -10557,10 +10617,10 @@
         <v>96</v>
       </c>
       <c r="C74" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D74" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -10571,10 +10631,10 @@
         <v>97</v>
       </c>
       <c r="C75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D75" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -10585,13 +10645,13 @@
         <v>100</v>
       </c>
       <c r="C77" t="s">
+        <v>425</v>
+      </c>
+      <c r="D77" t="s">
         <v>426</v>
       </c>
-      <c r="D77" t="s">
-        <v>427</v>
-      </c>
       <c r="E77" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -10611,7 +10671,7 @@
         <v>330</v>
       </c>
       <c r="F78" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -10631,7 +10691,7 @@
         <v>331</v>
       </c>
       <c r="F79" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -10642,10 +10702,10 @@
         <v>103</v>
       </c>
       <c r="C80" t="s">
+        <v>420</v>
+      </c>
+      <c r="D80" t="s">
         <v>421</v>
-      </c>
-      <c r="D80" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -10656,10 +10716,10 @@
         <v>104</v>
       </c>
       <c r="C81" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D81" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -10670,10 +10730,10 @@
         <v>105</v>
       </c>
       <c r="C82" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D82" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -10684,10 +10744,10 @@
         <v>106</v>
       </c>
       <c r="C83" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D83" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -10698,13 +10758,13 @@
         <v>101</v>
       </c>
       <c r="C84" t="s">
+        <v>425</v>
+      </c>
+      <c r="D84" t="s">
         <v>426</v>
       </c>
-      <c r="D84" t="s">
-        <v>427</v>
-      </c>
       <c r="E84" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -10715,10 +10775,10 @@
         <v>114</v>
       </c>
       <c r="C85" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D85" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -10729,10 +10789,10 @@
         <v>118</v>
       </c>
       <c r="C86" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D86" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E86" s="5"/>
     </row>
@@ -10744,10 +10804,10 @@
         <v>116</v>
       </c>
       <c r="C87" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D87" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -10758,10 +10818,10 @@
         <v>120</v>
       </c>
       <c r="C88" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D88" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -10772,10 +10832,10 @@
         <v>123</v>
       </c>
       <c r="C89" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D89" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -10786,10 +10846,10 @@
         <v>125</v>
       </c>
       <c r="E91" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F91" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -10800,10 +10860,10 @@
         <v>126</v>
       </c>
       <c r="E92" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F92" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -10814,10 +10874,10 @@
         <v>52</v>
       </c>
       <c r="C93" t="s">
+        <v>376</v>
+      </c>
+      <c r="D93" t="s">
         <v>377</v>
-      </c>
-      <c r="D93" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -10828,10 +10888,10 @@
         <v>53</v>
       </c>
       <c r="E94" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F94" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -10842,10 +10902,10 @@
         <v>127</v>
       </c>
       <c r="E95" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F95" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -10856,10 +10916,10 @@
         <v>129</v>
       </c>
       <c r="E96" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F96" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -10870,10 +10930,10 @@
         <v>130</v>
       </c>
       <c r="E97" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F97" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -10884,13 +10944,13 @@
         <v>56</v>
       </c>
       <c r="C98" t="s">
+        <v>381</v>
+      </c>
+      <c r="D98" t="s">
+        <v>380</v>
+      </c>
+      <c r="E98" t="s">
         <v>382</v>
-      </c>
-      <c r="D98" t="s">
-        <v>381</v>
-      </c>
-      <c r="E98" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -10901,10 +10961,10 @@
         <v>57</v>
       </c>
       <c r="E99" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F99" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -10915,13 +10975,13 @@
         <v>58</v>
       </c>
       <c r="C100" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D100" t="s">
         <v>213</v>
       </c>
       <c r="E100" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -10932,13 +10992,13 @@
         <v>59</v>
       </c>
       <c r="C101" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D101" t="s">
         <v>211</v>
       </c>
       <c r="E101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -10949,7 +11009,7 @@
         <v>63</v>
       </c>
       <c r="F102" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -10960,13 +11020,13 @@
         <v>68</v>
       </c>
       <c r="C103" t="s">
+        <v>387</v>
+      </c>
+      <c r="D103" t="s">
         <v>388</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>389</v>
-      </c>
-      <c r="E103" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -10977,10 +11037,10 @@
         <v>64</v>
       </c>
       <c r="C104" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D104" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -10991,13 +11051,13 @@
         <v>67</v>
       </c>
       <c r="C105" t="s">
+        <v>391</v>
+      </c>
+      <c r="D105" t="s">
         <v>392</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>393</v>
-      </c>
-      <c r="E105" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -11008,7 +11068,7 @@
         <v>65</v>
       </c>
       <c r="F106" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -11019,7 +11079,7 @@
         <v>66</v>
       </c>
       <c r="F107" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -11030,13 +11090,13 @@
         <v>135</v>
       </c>
       <c r="C108" t="s">
+        <v>433</v>
+      </c>
+      <c r="D108" t="s">
+        <v>432</v>
+      </c>
+      <c r="E108" t="s">
         <v>434</v>
-      </c>
-      <c r="D108" t="s">
-        <v>433</v>
-      </c>
-      <c r="E108" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -11047,10 +11107,10 @@
         <v>137</v>
       </c>
       <c r="C109" t="s">
+        <v>435</v>
+      </c>
+      <c r="D109" t="s">
         <v>436</v>
-      </c>
-      <c r="D109" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -11061,13 +11121,13 @@
         <v>71</v>
       </c>
       <c r="C110" t="s">
+        <v>395</v>
+      </c>
+      <c r="D110" t="s">
         <v>396</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>397</v>
-      </c>
-      <c r="E110" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -11078,10 +11138,10 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
+        <v>363</v>
+      </c>
+      <c r="D111" t="s">
         <v>364</v>
-      </c>
-      <c r="D111" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -11092,10 +11152,10 @@
         <v>32</v>
       </c>
       <c r="C112" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D112" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -11106,10 +11166,10 @@
         <v>33</v>
       </c>
       <c r="C113" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D113" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -11120,10 +11180,10 @@
         <v>34</v>
       </c>
       <c r="C114" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D114" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E114" t="s">
         <v>293</v>
@@ -11137,10 +11197,10 @@
         <v>35</v>
       </c>
       <c r="C115" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D115" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -11151,10 +11211,10 @@
         <v>36</v>
       </c>
       <c r="C116" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D116" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -11165,7 +11225,7 @@
         <v>37</v>
       </c>
       <c r="E117" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -11176,7 +11236,7 @@
         <v>38</v>
       </c>
       <c r="E118" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -11187,7 +11247,7 @@
         <v>39</v>
       </c>
       <c r="F119" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -11198,10 +11258,10 @@
         <v>40</v>
       </c>
       <c r="C120" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D120" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -11212,10 +11272,10 @@
         <v>72</v>
       </c>
       <c r="C121" t="s">
+        <v>437</v>
+      </c>
+      <c r="D121" t="s">
         <v>438</v>
-      </c>
-      <c r="D121" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -11285,13 +11345,13 @@
         <v>77</v>
       </c>
       <c r="C126" t="s">
+        <v>398</v>
+      </c>
+      <c r="D126" t="s">
+        <v>398</v>
+      </c>
+      <c r="E126" t="s">
         <v>399</v>
-      </c>
-      <c r="D126" t="s">
-        <v>399</v>
-      </c>
-      <c r="E126" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -11302,10 +11362,10 @@
         <v>323</v>
       </c>
       <c r="C127" t="s">
+        <v>400</v>
+      </c>
+      <c r="D127" t="s">
         <v>401</v>
-      </c>
-      <c r="D127" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -11316,16 +11376,16 @@
         <v>144</v>
       </c>
       <c r="C128" t="s">
+        <v>407</v>
+      </c>
+      <c r="D128" t="s">
         <v>408</v>
       </c>
-      <c r="D128" t="s">
-        <v>409</v>
-      </c>
       <c r="E128" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F128" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -11336,13 +11396,13 @@
         <v>145</v>
       </c>
       <c r="C129" t="s">
+        <v>440</v>
+      </c>
+      <c r="D129" t="s">
         <v>441</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" t="s">
         <v>442</v>
-      </c>
-      <c r="E129" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -11353,10 +11413,10 @@
         <v>146</v>
       </c>
       <c r="C130" t="s">
+        <v>443</v>
+      </c>
+      <c r="D130" t="s">
         <v>444</v>
-      </c>
-      <c r="D130" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -11367,13 +11427,13 @@
         <v>147</v>
       </c>
       <c r="C131" t="s">
+        <v>407</v>
+      </c>
+      <c r="D131" t="s">
         <v>408</v>
       </c>
-      <c r="D131" t="s">
-        <v>409</v>
-      </c>
       <c r="E131" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -11384,10 +11444,10 @@
         <v>126</v>
       </c>
       <c r="E133" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F133" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -11398,10 +11458,10 @@
         <v>52</v>
       </c>
       <c r="C134" t="s">
+        <v>376</v>
+      </c>
+      <c r="D134" t="s">
         <v>377</v>
-      </c>
-      <c r="D134" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -11412,10 +11472,10 @@
         <v>53</v>
       </c>
       <c r="E135" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F135" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -11426,10 +11486,10 @@
         <v>127</v>
       </c>
       <c r="E136" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F136" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -11440,10 +11500,10 @@
         <v>129</v>
       </c>
       <c r="E137" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F137" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -11454,10 +11514,10 @@
         <v>130</v>
       </c>
       <c r="E138" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F138" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -11468,13 +11528,13 @@
         <v>56</v>
       </c>
       <c r="C139" t="s">
+        <v>381</v>
+      </c>
+      <c r="D139" t="s">
+        <v>380</v>
+      </c>
+      <c r="E139" t="s">
         <v>382</v>
-      </c>
-      <c r="D139" t="s">
-        <v>381</v>
-      </c>
-      <c r="E139" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -11485,10 +11545,10 @@
         <v>57</v>
       </c>
       <c r="E140" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F140" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -11499,13 +11559,13 @@
         <v>58</v>
       </c>
       <c r="C141" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D141" t="s">
         <v>213</v>
       </c>
       <c r="E141" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -11516,13 +11576,13 @@
         <v>59</v>
       </c>
       <c r="C142" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D142" t="s">
         <v>211</v>
       </c>
       <c r="E142" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -11533,7 +11593,7 @@
         <v>63</v>
       </c>
       <c r="F143" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -11544,13 +11604,13 @@
         <v>68</v>
       </c>
       <c r="C144" t="s">
+        <v>387</v>
+      </c>
+      <c r="D144" t="s">
         <v>388</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" t="s">
         <v>389</v>
-      </c>
-      <c r="E144" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -11561,10 +11621,10 @@
         <v>64</v>
       </c>
       <c r="C145" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D145" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -11575,13 +11635,13 @@
         <v>67</v>
       </c>
       <c r="C146" t="s">
+        <v>391</v>
+      </c>
+      <c r="D146" t="s">
         <v>392</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>393</v>
-      </c>
-      <c r="E146" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -11592,7 +11652,7 @@
         <v>65</v>
       </c>
       <c r="F147" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -11603,7 +11663,7 @@
         <v>66</v>
       </c>
       <c r="F148" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -11614,13 +11674,13 @@
         <v>135</v>
       </c>
       <c r="C149" t="s">
+        <v>433</v>
+      </c>
+      <c r="D149" t="s">
+        <v>432</v>
+      </c>
+      <c r="E149" t="s">
         <v>434</v>
-      </c>
-      <c r="D149" t="s">
-        <v>433</v>
-      </c>
-      <c r="E149" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -11631,10 +11691,10 @@
         <v>137</v>
       </c>
       <c r="C150" t="s">
+        <v>435</v>
+      </c>
+      <c r="D150" t="s">
         <v>436</v>
-      </c>
-      <c r="D150" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -11645,13 +11705,13 @@
         <v>71</v>
       </c>
       <c r="C151" t="s">
+        <v>395</v>
+      </c>
+      <c r="D151" t="s">
         <v>396</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" t="s">
         <v>397</v>
-      </c>
-      <c r="E151" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -11662,10 +11722,10 @@
         <v>31</v>
       </c>
       <c r="C152" t="s">
+        <v>363</v>
+      </c>
+      <c r="D152" t="s">
         <v>364</v>
-      </c>
-      <c r="D152" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -11676,10 +11736,10 @@
         <v>32</v>
       </c>
       <c r="C153" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D153" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -11690,10 +11750,10 @@
         <v>33</v>
       </c>
       <c r="C154" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D154" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -11704,10 +11764,10 @@
         <v>34</v>
       </c>
       <c r="C155" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D155" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E155" t="s">
         <v>293</v>
@@ -11721,10 +11781,10 @@
         <v>35</v>
       </c>
       <c r="C156" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D156" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -11735,10 +11795,10 @@
         <v>36</v>
       </c>
       <c r="C157" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D157" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -11749,7 +11809,7 @@
         <v>37</v>
       </c>
       <c r="E158" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -11760,7 +11820,7 @@
         <v>38</v>
       </c>
       <c r="E159" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -11771,7 +11831,7 @@
         <v>39</v>
       </c>
       <c r="F160" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -11782,10 +11842,10 @@
         <v>40</v>
       </c>
       <c r="C161" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D161" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -11796,10 +11856,10 @@
         <v>72</v>
       </c>
       <c r="C162" t="s">
+        <v>437</v>
+      </c>
+      <c r="D162" t="s">
         <v>438</v>
-      </c>
-      <c r="D162" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -11869,13 +11929,13 @@
         <v>77</v>
       </c>
       <c r="C167" t="s">
+        <v>398</v>
+      </c>
+      <c r="D167" t="s">
+        <v>398</v>
+      </c>
+      <c r="E167" t="s">
         <v>399</v>
-      </c>
-      <c r="D167" t="s">
-        <v>399</v>
-      </c>
-      <c r="E167" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -11886,10 +11946,10 @@
         <v>323</v>
       </c>
       <c r="C168" t="s">
+        <v>400</v>
+      </c>
+      <c r="D168" t="s">
         <v>401</v>
-      </c>
-      <c r="D168" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -11900,10 +11960,10 @@
         <v>150</v>
       </c>
       <c r="C169" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D169" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -11914,10 +11974,10 @@
         <v>151</v>
       </c>
       <c r="C170" t="s">
+        <v>452</v>
+      </c>
+      <c r="D170" t="s">
         <v>453</v>
-      </c>
-      <c r="D170" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -11928,13 +11988,13 @@
         <v>152</v>
       </c>
       <c r="C171" t="s">
+        <v>454</v>
+      </c>
+      <c r="D171" t="s">
         <v>455</v>
       </c>
-      <c r="D171" t="s">
+      <c r="E171" t="s">
         <v>456</v>
-      </c>
-      <c r="E171" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -11945,13 +12005,13 @@
         <v>153</v>
       </c>
       <c r="C172" t="s">
+        <v>457</v>
+      </c>
+      <c r="D172" t="s">
         <v>458</v>
       </c>
-      <c r="D172" t="s">
+      <c r="E172" t="s">
         <v>459</v>
-      </c>
-      <c r="E172" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -11962,7 +12022,7 @@
         <v>156</v>
       </c>
       <c r="F173" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -11970,10 +12030,10 @@
         <v>149</v>
       </c>
       <c r="B174" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F174" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -11984,19 +12044,19 @@
         <v>157</v>
       </c>
       <c r="C175" t="s">
+        <v>460</v>
+      </c>
+      <c r="D175" t="s">
+        <v>357</v>
+      </c>
+      <c r="E175" t="s">
         <v>461</v>
       </c>
-      <c r="D175" t="s">
-        <v>358</v>
-      </c>
-      <c r="E175" t="s">
-        <v>462</v>
-      </c>
       <c r="F175" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G175" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -12007,7 +12067,7 @@
         <v>159</v>
       </c>
       <c r="C176" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D176" t="s">
         <v>228</v>
@@ -12021,7 +12081,7 @@
         <v>158</v>
       </c>
       <c r="C177" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D177" t="s">
         <v>228</v>
@@ -12035,7 +12095,7 @@
         <v>160</v>
       </c>
       <c r="C178" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D178" t="s">
         <v>228</v>
@@ -12049,13 +12109,13 @@
         <v>161</v>
       </c>
       <c r="C179" t="s">
+        <v>466</v>
+      </c>
+      <c r="D179" t="s">
         <v>467</v>
       </c>
-      <c r="D179" t="s">
+      <c r="E179" t="s">
         <v>468</v>
-      </c>
-      <c r="E179" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -12066,10 +12126,10 @@
         <v>126</v>
       </c>
       <c r="E181" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F181" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -12080,10 +12140,10 @@
         <v>52</v>
       </c>
       <c r="C182" t="s">
+        <v>376</v>
+      </c>
+      <c r="D182" t="s">
         <v>377</v>
-      </c>
-      <c r="D182" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -12094,10 +12154,10 @@
         <v>53</v>
       </c>
       <c r="E183" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F183" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -12108,10 +12168,10 @@
         <v>127</v>
       </c>
       <c r="E184" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F184" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -12122,10 +12182,10 @@
         <v>129</v>
       </c>
       <c r="E185" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F185" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -12136,10 +12196,10 @@
         <v>130</v>
       </c>
       <c r="E186" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F186" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -12150,13 +12210,13 @@
         <v>56</v>
       </c>
       <c r="C187" t="s">
+        <v>381</v>
+      </c>
+      <c r="D187" t="s">
+        <v>380</v>
+      </c>
+      <c r="E187" t="s">
         <v>382</v>
-      </c>
-      <c r="D187" t="s">
-        <v>381</v>
-      </c>
-      <c r="E187" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -12167,10 +12227,10 @@
         <v>57</v>
       </c>
       <c r="E188" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F188" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -12181,13 +12241,13 @@
         <v>58</v>
       </c>
       <c r="C189" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D189" t="s">
         <v>213</v>
       </c>
       <c r="E189" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -12198,13 +12258,13 @@
         <v>59</v>
       </c>
       <c r="C190" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D190" t="s">
         <v>211</v>
       </c>
       <c r="E190" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -12215,7 +12275,7 @@
         <v>63</v>
       </c>
       <c r="F191" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -12226,13 +12286,13 @@
         <v>68</v>
       </c>
       <c r="C192" t="s">
+        <v>387</v>
+      </c>
+      <c r="D192" t="s">
         <v>388</v>
       </c>
-      <c r="D192" t="s">
+      <c r="E192" t="s">
         <v>389</v>
-      </c>
-      <c r="E192" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -12243,10 +12303,10 @@
         <v>64</v>
       </c>
       <c r="C193" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D193" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -12257,13 +12317,13 @@
         <v>67</v>
       </c>
       <c r="C194" t="s">
+        <v>391</v>
+      </c>
+      <c r="D194" t="s">
         <v>392</v>
       </c>
-      <c r="D194" t="s">
+      <c r="E194" t="s">
         <v>393</v>
-      </c>
-      <c r="E194" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -12274,7 +12334,7 @@
         <v>65</v>
       </c>
       <c r="F195" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -12285,7 +12345,7 @@
         <v>66</v>
       </c>
       <c r="F196" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -12296,13 +12356,13 @@
         <v>135</v>
       </c>
       <c r="C197" t="s">
+        <v>433</v>
+      </c>
+      <c r="D197" t="s">
+        <v>432</v>
+      </c>
+      <c r="E197" t="s">
         <v>434</v>
-      </c>
-      <c r="D197" t="s">
-        <v>433</v>
-      </c>
-      <c r="E197" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -12313,10 +12373,10 @@
         <v>137</v>
       </c>
       <c r="C198" t="s">
+        <v>435</v>
+      </c>
+      <c r="D198" t="s">
         <v>436</v>
-      </c>
-      <c r="D198" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -12327,13 +12387,13 @@
         <v>71</v>
       </c>
       <c r="C199" t="s">
+        <v>395</v>
+      </c>
+      <c r="D199" t="s">
         <v>396</v>
       </c>
-      <c r="D199" t="s">
+      <c r="E199" t="s">
         <v>397</v>
-      </c>
-      <c r="E199" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -12344,10 +12404,10 @@
         <v>31</v>
       </c>
       <c r="C200" t="s">
+        <v>363</v>
+      </c>
+      <c r="D200" t="s">
         <v>364</v>
-      </c>
-      <c r="D200" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -12358,10 +12418,10 @@
         <v>32</v>
       </c>
       <c r="C201" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D201" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -12372,10 +12432,10 @@
         <v>33</v>
       </c>
       <c r="C202" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D202" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -12386,10 +12446,10 @@
         <v>34</v>
       </c>
       <c r="C203" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D203" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E203" t="s">
         <v>293</v>
@@ -12403,10 +12463,10 @@
         <v>35</v>
       </c>
       <c r="C204" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D204" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -12417,10 +12477,10 @@
         <v>36</v>
       </c>
       <c r="C205" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D205" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -12431,7 +12491,7 @@
         <v>37</v>
       </c>
       <c r="E206" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -12442,7 +12502,7 @@
         <v>38</v>
       </c>
       <c r="E207" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -12453,7 +12513,7 @@
         <v>39</v>
       </c>
       <c r="F208" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -12464,10 +12524,10 @@
         <v>40</v>
       </c>
       <c r="C209" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D209" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -12478,10 +12538,10 @@
         <v>72</v>
       </c>
       <c r="C210" t="s">
+        <v>437</v>
+      </c>
+      <c r="D210" t="s">
         <v>438</v>
-      </c>
-      <c r="D210" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -12551,13 +12611,13 @@
         <v>77</v>
       </c>
       <c r="C215" t="s">
+        <v>398</v>
+      </c>
+      <c r="D215" t="s">
+        <v>398</v>
+      </c>
+      <c r="E215" t="s">
         <v>399</v>
-      </c>
-      <c r="D215" t="s">
-        <v>399</v>
-      </c>
-      <c r="E215" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -12568,10 +12628,10 @@
         <v>323</v>
       </c>
       <c r="C216" t="s">
+        <v>400</v>
+      </c>
+      <c r="D216" t="s">
         <v>401</v>
-      </c>
-      <c r="D216" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -12582,10 +12642,10 @@
         <v>146</v>
       </c>
       <c r="C217" t="s">
+        <v>443</v>
+      </c>
+      <c r="D217" t="s">
         <v>444</v>
-      </c>
-      <c r="D217" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -12596,13 +12656,13 @@
         <v>147</v>
       </c>
       <c r="C218" t="s">
+        <v>407</v>
+      </c>
+      <c r="D218" t="s">
         <v>408</v>
       </c>
-      <c r="D218" t="s">
-        <v>409</v>
-      </c>
       <c r="E218" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -12613,10 +12673,10 @@
         <v>179</v>
       </c>
       <c r="C219" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D219" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -12624,13 +12684,13 @@
         <v>162</v>
       </c>
       <c r="B220" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C220" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D220" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -12641,7 +12701,7 @@
         <v>50</v>
       </c>
       <c r="E222" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -12652,7 +12712,7 @@
         <v>180</v>
       </c>
       <c r="E223" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -12663,7 +12723,7 @@
         <v>181</v>
       </c>
       <c r="E224" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -12707,7 +12767,7 @@
         <v>227</v>
       </c>
       <c r="D229" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -12715,13 +12775,13 @@
         <v>185</v>
       </c>
       <c r="B230" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C230" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D230" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -12735,7 +12795,7 @@
         <v>226</v>
       </c>
       <c r="D231" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -12746,7 +12806,7 @@
         <v>189</v>
       </c>
       <c r="E233" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -12757,7 +12817,7 @@
         <v>190</v>
       </c>
       <c r="E234" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -12768,13 +12828,13 @@
         <v>181</v>
       </c>
       <c r="C235" t="s">
+        <v>483</v>
+      </c>
+      <c r="D235" t="s">
         <v>484</v>
       </c>
-      <c r="D235" t="s">
-        <v>485</v>
-      </c>
       <c r="E235" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -12785,10 +12845,10 @@
         <v>192</v>
       </c>
       <c r="C236" t="s">
+        <v>481</v>
+      </c>
+      <c r="D236" t="s">
         <v>482</v>
-      </c>
-      <c r="D236" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Creacion de Carpetas en el Backend, Tablas TP, Carpeta Models, servicios con entidades
</commit_message>
<xml_diff>
--- a/Formulario - Base de datos.xlsx
+++ b/Formulario - Base de datos.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3130" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="493">
   <si>
     <t>Gobernacion maritima</t>
   </si>
@@ -1482,6 +1482,21 @@
   </si>
   <si>
     <t>Personas.PersonaNatural</t>
+  </si>
+  <si>
+    <t>falta campo</t>
+  </si>
+  <si>
+    <t>donde se ingresa el dato</t>
+  </si>
+  <si>
+    <t>falta campo, donde se ingresa el dato</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>personas a quien el niño conto hechos</t>
   </si>
 </sst>
 </file>
@@ -9570,8 +9585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9581,10 +9596,10 @@
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>273</v>
       </c>
@@ -9600,8 +9615,11 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>485</v>
       </c>
@@ -9612,7 +9630,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>485</v>
       </c>
@@ -9622,8 +9640,14 @@
       <c r="E3" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>445</v>
+      </c>
+      <c r="G3" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>485</v>
       </c>
@@ -9633,8 +9657,14 @@
       <c r="E4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>445</v>
+      </c>
+      <c r="G4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>485</v>
       </c>
@@ -9651,7 +9681,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>485</v>
       </c>
@@ -9668,7 +9698,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>485</v>
       </c>
@@ -9682,7 +9712,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>485</v>
       </c>
@@ -9696,7 +9726,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>485</v>
       </c>
@@ -9710,7 +9740,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>485</v>
       </c>
@@ -9727,7 +9757,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>485</v>
       </c>
@@ -9737,8 +9767,11 @@
       <c r="F11" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>274</v>
       </c>
@@ -9748,8 +9781,11 @@
       <c r="F13" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>274</v>
       </c>
@@ -9766,7 +9802,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>274</v>
       </c>
@@ -9783,7 +9819,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>274</v>
       </c>
@@ -9800,7 +9836,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>274</v>
       </c>
@@ -9817,7 +9853,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>274</v>
       </c>
@@ -9831,7 +9867,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>274</v>
       </c>
@@ -9845,7 +9881,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>274</v>
       </c>
@@ -9859,7 +9895,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>274</v>
       </c>
@@ -9876,7 +9912,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>274</v>
       </c>
@@ -9890,7 +9926,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>274</v>
       </c>
@@ -9904,7 +9940,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>274</v>
       </c>
@@ -9915,7 +9951,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>274</v>
       </c>
@@ -9926,7 +9962,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>274</v>
       </c>
@@ -9936,8 +9972,11 @@
       <c r="F26" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>274</v>
       </c>
@@ -9951,7 +9990,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>274</v>
       </c>
@@ -9965,7 +10004,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>274</v>
       </c>
@@ -9979,7 +10018,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -9992,8 +10031,11 @@
       <c r="F31" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -10007,7 +10049,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -10020,8 +10062,11 @@
       <c r="F33" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -10034,8 +10079,11 @@
       <c r="F34" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -10048,8 +10096,11 @@
       <c r="F35" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -10062,8 +10113,11 @@
       <c r="F36" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -10080,7 +10134,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -10093,8 +10147,11 @@
       <c r="F38" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -10111,7 +10168,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -10128,7 +10185,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -10144,8 +10201,11 @@
       <c r="F41" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -10162,7 +10222,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -10176,7 +10236,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -10193,7 +10253,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -10203,8 +10263,11 @@
       <c r="F45" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -10214,8 +10277,11 @@
       <c r="F46" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -10232,7 +10298,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -10246,7 +10312,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -10260,7 +10326,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -10274,7 +10340,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -10291,7 +10357,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -10305,7 +10371,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -10319,7 +10385,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -10330,7 +10396,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -10341,7 +10407,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -10351,8 +10417,11 @@
       <c r="F56" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -10366,7 +10435,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -10380,7 +10449,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -10397,7 +10466,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -10414,7 +10483,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -10431,7 +10500,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -10439,7 +10508,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -10456,7 +10525,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>49</v>
       </c>
@@ -10470,7 +10539,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -10487,7 +10556,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -10504,7 +10573,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -10518,7 +10587,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -10537,13 +10606,16 @@
       <c r="F68" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>492</v>
       </c>
       <c r="C69" t="s">
         <v>326</v>
@@ -10557,8 +10629,11 @@
       <c r="F69" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -10577,8 +10652,11 @@
       <c r="F70" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -10595,7 +10673,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -10609,7 +10687,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>93</v>
       </c>
@@ -10623,7 +10701,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>93</v>
       </c>
@@ -10637,7 +10715,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>329</v>
       </c>
@@ -10654,7 +10732,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>329</v>
       </c>
@@ -10674,7 +10752,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>329</v>
       </c>
@@ -10694,7 +10772,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>329</v>
       </c>

</xml_diff>